<commit_message>
random menu cost appears to be functional, though slow
</commit_message>
<xml_diff>
--- a/output/run3_table.xlsx
+++ b/output/run3_table.xlsx
@@ -13,7 +13,442 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="435">
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>beta (annualized)</t>
+  </si>
+  <si>
+    <t>____Income Statistics</t>
+  </si>
+  <si>
+    <t>Mean gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log net annual income</t>
+  </si>
+  <si>
+    <t>____Wealth Statistics</t>
+  </si>
+  <si>
+    <t>Mean total wealth</t>
+  </si>
+  <si>
+    <t>Mean liquid wealth</t>
+  </si>
+  <si>
+    <t>w, median</t>
+  </si>
+  <si>
+    <t>b, median</t>
+  </si>
+  <si>
+    <t>s = 0</t>
+  </si>
+  <si>
+    <t>b &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 15% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= $500</t>
+  </si>
+  <si>
+    <t>b &lt;= $1000</t>
+  </si>
+  <si>
+    <t>b &lt;= $2000</t>
+  </si>
+  <si>
+    <t>b &lt;= $5000</t>
+  </si>
+  <si>
+    <t>b &lt;= $10000</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/6</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/12</t>
+  </si>
+  <si>
+    <t>w, Top 10% share</t>
+  </si>
+  <si>
+    <t>w, Top 1% share</t>
+  </si>
+  <si>
+    <t>Gini coefficient, wealth</t>
+  </si>
+  <si>
+    <t>____MPC size effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____MPC sign effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>____MPC for HtM households</t>
+  </si>
+  <si>
+    <t>Quarterly  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>____Wealth percentiles</t>
+  </si>
+  <si>
+    <t>w, 10th pctile</t>
+  </si>
+  <si>
+    <t>w, 25th pctile</t>
+  </si>
+  <si>
+    <t>w, 50th pctile</t>
+  </si>
+  <si>
+    <t>w, 90th pctile</t>
+  </si>
+  <si>
+    <t>w, 95th pctile</t>
+  </si>
+  <si>
+    <t>w, 98th pctile</t>
+  </si>
+  <si>
+    <t>w, 99th pctile</t>
+  </si>
+  <si>
+    <t>w, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Liquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>b, 10th pctile</t>
+  </si>
+  <si>
+    <t>b, 25th pctile</t>
+  </si>
+  <si>
+    <t>b, 50th pctile</t>
+  </si>
+  <si>
+    <t>b, 90th pctile</t>
+  </si>
+  <si>
+    <t>b, 95th pctile</t>
+  </si>
+  <si>
+    <t>b, 98th pctile</t>
+  </si>
+  <si>
+    <t>b, 99th pctile</t>
+  </si>
+  <si>
+    <t>b, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>a, 10th pctile</t>
+  </si>
+  <si>
+    <t>a, 25th pctile</t>
+  </si>
+  <si>
+    <t>a, 50th pctile</t>
+  </si>
+  <si>
+    <t>a, 90th pctile</t>
+  </si>
+  <si>
+    <t>a, 95th pctile</t>
+  </si>
+  <si>
+    <t>a, 98th pctile</t>
+  </si>
+  <si>
+    <t>a, 99th pctile</t>
+  </si>
+  <si>
+    <t>a, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid mpcs</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____Adjustment cost statistics,cost(d,a) =k0 * |d| + k1 * |d| ^ (1 + k2) / (1 + k2)</t>
+  </si>
+  <si>
+    <t>kappa0, adj cost coeff on first (linear) term</t>
+  </si>
+  <si>
+    <t>kappa1, adj cost coeff on second (power) term</t>
+  </si>
+  <si>
+    <t>kappa2, power on second term</t>
+  </si>
+  <si>
+    <t>kappa1 ^(-1/kappa2), low values cause mass at high a</t>
+  </si>
+  <si>
+    <t>a_lb, parameter s.t. max(a, a_lb) used for adj cost</t>
+  </si>
+  <si>
+    <t>Mean adjustment cost, E[chi(d, a)]</t>
+  </si>
+  <si>
+    <t>Mean ratio of deposits to assets, E[|d| / max(a, a_lb)]</t>
+  </si>
+  <si>
+    <t>E[chi(d,a)/abs(d) | d != 0]</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 10th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 25th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 50th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 90th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 95th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 99th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>____Other parameters</t>
+  </si>
+  <si>
+    <t>Experiment group no.</t>
+  </si>
+  <si>
+    <t>Liquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Illiquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Death rate (quarterly)</t>
+  </si>
+  <si>
+    <t>Bequests, on or off</t>
+  </si>
+  <si>
+    <t>Max liquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Max illiquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Borrowing limit</t>
+  </si>
+  <si>
+    <t>CRRA coefficient</t>
+  </si>
+  <si>
+    <t>Value of the numeraire, mean annual earning, in $</t>
+  </si>
+  <si>
+    <t>Income Process</t>
+  </si>
+  <si>
+    <t>____Other statistics</t>
+  </si>
+  <si>
+    <t>a &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= $500</t>
+  </si>
+  <si>
+    <t>a &lt;= $1000</t>
+  </si>
+  <si>
+    <t>a &lt;= $2000</t>
+  </si>
+  <si>
+    <t>a &lt;= $5000</t>
+  </si>
+  <si>
+    <t>a &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= $500</t>
+  </si>
+  <si>
+    <t>w &lt;= $1000</t>
+  </si>
+  <si>
+    <t>w &lt;= $2000</t>
+  </si>
+  <si>
+    <t>w &lt;= $5000</t>
+  </si>
+  <si>
+    <t>w &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>Specification1</t>
+  </si>
+  <si>
+    <t>iy=1, kappa2=0.25</t>
+  </si>
+  <si>
+    <t>cont_a, no meas err</t>
+  </si>
   <si>
     <t>Row</t>
   </si>
@@ -903,7 +1338,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -913,14 +1348,16 @@
     </border>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -939,39 +1376,39 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>145</v>
+        <v>290</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>287</v>
+        <v>432</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>146</v>
+        <v>291</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>288</v>
+        <v>433</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>147</v>
+        <v>292</v>
       </c>
       <c r="B3" s="0">
-        <v>8.7285132994258721</v>
+        <v>8.7285132994264512</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>148</v>
+        <v>293</v>
       </c>
       <c r="B4" s="0">
-        <v>23.920912670565098</v>
+        <v>23.920912670566707</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>149</v>
+        <v>294</v>
       </c>
       <c r="B5" s="0">
         <v>0.98019867330675525</v>
@@ -979,13 +1416,13 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>150</v>
+        <v>295</v>
       </c>
       <c r="B6" s="0"/>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>151</v>
+        <v>296</v>
       </c>
       <c r="B7" s="0">
         <v>1.0691087245941162</v>
@@ -993,7 +1430,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>152</v>
+        <v>297</v>
       </c>
       <c r="B8" s="0">
         <v>0.77865374088287354</v>
@@ -1001,7 +1438,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>153</v>
+        <v>298</v>
       </c>
       <c r="B9" s="0">
         <v>0.77865374088287354</v>
@@ -1009,497 +1446,497 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>154</v>
+        <v>299</v>
       </c>
       <c r="B10" s="0"/>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>155</v>
+        <v>300</v>
       </c>
       <c r="B11" s="0">
-        <v>0.81138036092355981</v>
+        <v>0.81138036092356036</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>156</v>
+        <v>301</v>
       </c>
       <c r="B12" s="0">
-        <v>0.81088099507740585</v>
+        <v>0.81088099507740774</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>157</v>
+        <v>302</v>
       </c>
       <c r="B13" s="0">
-        <v>0.22694281077739045</v>
+        <v>0.22694281077739129</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>158</v>
+        <v>303</v>
       </c>
       <c r="B14" s="0">
-        <v>0.18989735697904109</v>
+        <v>0.18989735697904642</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>159</v>
+        <v>304</v>
       </c>
       <c r="B15" s="0">
-        <v>0.23749110138382992</v>
+        <v>0.23749110138386587</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>160</v>
+        <v>305</v>
       </c>
       <c r="B16" s="0">
-        <v>0.05798936885848003</v>
+        <v>0.057989368858519096</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>161</v>
+        <v>306</v>
       </c>
       <c r="B17" s="0">
-        <v>0.11082803850542447</v>
+        <v>0.11082803850547124</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>162</v>
+        <v>307</v>
       </c>
       <c r="B18" s="0">
-        <v>0.15314978285987477</v>
+        <v>0.15314978285992428</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>163</v>
+        <v>308</v>
       </c>
       <c r="B19" s="0">
-        <v>0.20042031734191204</v>
+        <v>0.20042031734194862</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>164</v>
+        <v>309</v>
       </c>
       <c r="B20" s="0">
-        <v>0.29728632729764265</v>
+        <v>0.29728632729763427</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>165</v>
+        <v>310</v>
       </c>
       <c r="B21" s="0">
-        <v>0.39040564336828626</v>
+        <v>0.39040564336825689</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>166</v>
+        <v>311</v>
       </c>
       <c r="B22" s="0">
-        <v>0.45969393975675632</v>
+        <v>0.45969393975673728</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>167</v>
+        <v>312</v>
       </c>
       <c r="B23" s="0">
-        <v>0.13422440508930461</v>
+        <v>0.1342244050893541</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>168</v>
+        <v>313</v>
       </c>
       <c r="B24" s="0">
-        <v>0.17754458123364383</v>
+        <v>0.17754458123368744</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>169</v>
+        <v>314</v>
       </c>
       <c r="B25" s="0">
-        <v>0.23842040534138351</v>
+        <v>0.23842040534140532</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>170</v>
+        <v>315</v>
       </c>
       <c r="B26" s="0">
-        <v>0.34708921160909639</v>
+        <v>0.34708921160906692</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>171</v>
+        <v>316</v>
       </c>
       <c r="B27" s="0">
-        <v>0.45843989528416518</v>
+        <v>0.45843989528414586</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>172</v>
+        <v>317</v>
       </c>
       <c r="B28" s="0">
-        <v>0.15610826301591232</v>
+        <v>0.1561082630159637</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>173</v>
+        <v>318</v>
       </c>
       <c r="B29" s="0">
-        <v>0.098206497818360147</v>
+        <v>0.098206497818401323</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>174</v>
+        <v>319</v>
       </c>
       <c r="B30" s="0">
-        <v>0.0065138118939700451</v>
+        <v>0.0065138118939686018</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>175</v>
+        <v>320</v>
       </c>
       <c r="B31" s="0">
-        <v>0.0086474583207197808</v>
+        <v>0.0086474583207147848</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>176</v>
+        <v>321</v>
       </c>
       <c r="B32" s="0">
-        <v>0.49770029962152817</v>
+        <v>0.49770029962151197</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>177</v>
+        <v>322</v>
       </c>
       <c r="B33" s="0">
-        <v>0.10903998460942155</v>
+        <v>0.10903998460942077</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>178</v>
+        <v>323</v>
       </c>
       <c r="B34" s="0">
-        <v>0.67019544887908611</v>
+        <v>0.67019544887908689</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>179</v>
+        <v>324</v>
       </c>
       <c r="B35" s="0"/>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>180</v>
+        <v>325</v>
       </c>
       <c r="B36" s="0">
-        <v>8.7285132994442218</v>
+        <v>8.7285132994463588</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>181</v>
+        <v>326</v>
       </c>
       <c r="B37" s="0">
-        <v>7.0820274460317041</v>
+        <v>7.0820274460317743</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>182</v>
+        <v>327</v>
       </c>
       <c r="B38" s="0">
-        <v>23.920912670580957</v>
+        <v>23.920912670588404</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>183</v>
+        <v>328</v>
       </c>
       <c r="B39" s="0">
-        <v>22.524652684369677</v>
+        <v>22.524652684370228</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>184</v>
+        <v>329</v>
       </c>
       <c r="B40" s="0"/>
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>185</v>
+        <v>330</v>
       </c>
       <c r="B41" s="0">
-        <v>15.622825160212223</v>
+        <v>15.622825160200909</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>186</v>
+        <v>331</v>
       </c>
       <c r="B42" s="0">
-        <v>15.62282516019865</v>
+        <v>15.622825160195298</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>187</v>
+        <v>332</v>
       </c>
       <c r="B43" s="0">
-        <v>21.500324605082152</v>
+        <v>21.500324605083986</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>188</v>
+        <v>333</v>
       </c>
       <c r="B44" s="0">
-        <v>33.74178251972851</v>
+        <v>33.741782519713013</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>189</v>
+        <v>334</v>
       </c>
       <c r="B45" s="0">
-        <v>33.741782519705382</v>
+        <v>33.741782519700969</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>190</v>
+        <v>335</v>
       </c>
       <c r="B46" s="0">
-        <v>36.881961318848212</v>
+        <v>36.88196131884856</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>191</v>
+        <v>336</v>
       </c>
       <c r="B47" s="0"/>
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>192</v>
+        <v>337</v>
       </c>
       <c r="B48" s="0">
-        <v>28.679518103852253</v>
+        <v>28.679518103847833</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>193</v>
+        <v>338</v>
       </c>
       <c r="B49" s="0">
-        <v>28.287209478122417</v>
+        <v>28.287209478128812</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>194</v>
+        <v>339</v>
       </c>
       <c r="B50" s="0">
-        <v>28.67969057382081</v>
+        <v>28.679690573816398</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>195</v>
+        <v>340</v>
       </c>
       <c r="B51" s="0">
-        <v>53.296321179569873</v>
+        <v>53.296321179570924</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>196</v>
+        <v>341</v>
       </c>
       <c r="B52" s="0">
-        <v>51.898352806466704</v>
+        <v>51.898352806477966</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>197</v>
+        <v>342</v>
       </c>
       <c r="B53" s="0">
-        <v>53.296935766009071</v>
+        <v>53.296935766010137</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>198</v>
+        <v>343</v>
       </c>
       <c r="B54" s="0"/>
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>199</v>
+        <v>344</v>
       </c>
       <c r="B55" s="0">
-        <v>0.0029635246545208194</v>
+        <v>0.0029635246545148494</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>200</v>
+        <v>345</v>
       </c>
       <c r="B56" s="0">
-        <v>0.02186929484533208</v>
+        <v>0.021869294845328346</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>201</v>
+        <v>346</v>
       </c>
       <c r="B57" s="0">
-        <v>0.22694281077739045</v>
+        <v>0.22694281077739129</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>202</v>
+        <v>347</v>
       </c>
       <c r="B58" s="0">
-        <v>1.7430834237500101</v>
+        <v>1.743083423750011</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>203</v>
+        <v>348</v>
       </c>
       <c r="B59" s="0">
-        <v>2.7389698883246676</v>
+        <v>2.7389698883246605</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>204</v>
+        <v>349</v>
       </c>
       <c r="B60" s="0">
-        <v>5.5530515937904985</v>
+        <v>5.5530515937904967</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>205</v>
+        <v>350</v>
       </c>
       <c r="B61" s="0">
-        <v>5.6482333471432824</v>
+        <v>5.6482333471432691</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>206</v>
+        <v>351</v>
       </c>
       <c r="B62" s="0">
-        <v>12.859337972504461</v>
+        <v>12.859337972504475</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
-        <v>207</v>
+        <v>352</v>
       </c>
       <c r="B63" s="0"/>
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
-        <v>208</v>
+        <v>353</v>
       </c>
       <c r="B64" s="0">
-        <v>0.0029606024109503516</v>
+        <v>0.0029606024109443954</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
-        <v>209</v>
+        <v>354</v>
       </c>
       <c r="B65" s="0">
-        <v>0.034326090628112815</v>
+        <v>0.034326090628109804</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">
-        <v>210</v>
+        <v>355</v>
       </c>
       <c r="B66" s="0">
-        <v>0.18989735697904109</v>
+        <v>0.18989735697904642</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="s">
-        <v>211</v>
+        <v>356</v>
       </c>
       <c r="B67" s="0">
-        <v>1.7247213493765303</v>
+        <v>1.7247213493765416</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
-        <v>212</v>
+        <v>357</v>
       </c>
       <c r="B68" s="0">
-        <v>2.7281765775996254</v>
+        <v>2.7281765775996458</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="s">
-        <v>213</v>
+        <v>358</v>
       </c>
       <c r="B69" s="0">
-        <v>4.2636404013217106</v>
+        <v>4.2636404013217497</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="s">
-        <v>214</v>
+        <v>359</v>
       </c>
       <c r="B70" s="0">
-        <v>5.5685675406639525</v>
+        <v>5.5685675406640334</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="s">
-        <v>215</v>
+        <v>360</v>
       </c>
       <c r="B71" s="0">
-        <v>10.269739239515065</v>
+        <v>10.269739239515749</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
-        <v>216</v>
+        <v>361</v>
       </c>
       <c r="B72" s="0"/>
     </row>
     <row r="73">
       <c r="A73" s="0" t="s">
-        <v>217</v>
+        <v>362</v>
       </c>
       <c r="B73" s="0">
         <v>0</v>
@@ -1507,7 +1944,7 @@
     </row>
     <row r="74">
       <c r="A74" s="0" t="s">
-        <v>218</v>
+        <v>363</v>
       </c>
       <c r="B74" s="0">
         <v>0</v>
@@ -1515,7 +1952,7 @@
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
-        <v>219</v>
+        <v>364</v>
       </c>
       <c r="B75" s="0">
         <v>0</v>
@@ -1523,7 +1960,7 @@
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
-        <v>220</v>
+        <v>365</v>
       </c>
       <c r="B76" s="0">
         <v>0</v>
@@ -1531,7 +1968,7 @@
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
-        <v>221</v>
+        <v>366</v>
       </c>
       <c r="B77" s="0">
         <v>0</v>
@@ -1539,7 +1976,7 @@
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
-        <v>222</v>
+        <v>367</v>
       </c>
       <c r="B78" s="0">
         <v>0</v>
@@ -1547,7 +1984,7 @@
     </row>
     <row r="79">
       <c r="A79" s="0" t="s">
-        <v>223</v>
+        <v>368</v>
       </c>
       <c r="B79" s="0">
         <v>0</v>
@@ -1555,81 +1992,81 @@
     </row>
     <row r="80">
       <c r="A80" s="0" t="s">
-        <v>224</v>
+        <v>369</v>
       </c>
       <c r="B80" s="0">
-        <v>0.021412439236154691</v>
+        <v>0.021412439236011851</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="s">
-        <v>225</v>
+        <v>370</v>
       </c>
       <c r="B81" s="0"/>
     </row>
     <row r="82">
       <c r="A82" s="0" t="s">
-        <v>226</v>
+        <v>371</v>
       </c>
       <c r="B82" s="0"/>
     </row>
     <row r="83">
       <c r="A83" s="0" t="s">
-        <v>227</v>
+        <v>372</v>
       </c>
       <c r="B83" s="0"/>
     </row>
     <row r="84">
       <c r="A84" s="0" t="s">
-        <v>228</v>
+        <v>373</v>
       </c>
       <c r="B84" s="0"/>
     </row>
     <row r="85">
       <c r="A85" s="0" t="s">
-        <v>229</v>
+        <v>374</v>
       </c>
       <c r="B85" s="0"/>
     </row>
     <row r="86">
       <c r="A86" s="0" t="s">
-        <v>230</v>
+        <v>375</v>
       </c>
       <c r="B86" s="0"/>
     </row>
     <row r="87">
       <c r="A87" s="0" t="s">
-        <v>231</v>
+        <v>376</v>
       </c>
       <c r="B87" s="0"/>
     </row>
     <row r="88">
       <c r="A88" s="0" t="s">
-        <v>232</v>
+        <v>377</v>
       </c>
       <c r="B88" s="0"/>
     </row>
     <row r="89">
       <c r="A89" s="0" t="s">
-        <v>233</v>
+        <v>378</v>
       </c>
       <c r="B89" s="0"/>
     </row>
     <row r="90">
       <c r="A90" s="0" t="s">
-        <v>234</v>
+        <v>379</v>
       </c>
       <c r="B90" s="0"/>
     </row>
     <row r="91">
       <c r="A91" s="0" t="s">
-        <v>235</v>
+        <v>380</v>
       </c>
       <c r="B91" s="0"/>
     </row>
     <row r="92">
       <c r="A92" s="0" t="s">
-        <v>236</v>
+        <v>381</v>
       </c>
       <c r="B92" s="0">
         <v>0</v>
@@ -1637,7 +2074,7 @@
     </row>
     <row r="93">
       <c r="A93" s="0" t="s">
-        <v>237</v>
+        <v>382</v>
       </c>
       <c r="B93" s="0">
         <v>0.60000000000000009</v>
@@ -1645,7 +2082,7 @@
     </row>
     <row r="94">
       <c r="A94" s="0" t="s">
-        <v>238</v>
+        <v>383</v>
       </c>
       <c r="B94" s="0">
         <v>0.25</v>
@@ -1653,7 +2090,7 @@
     </row>
     <row r="95">
       <c r="A95" s="0" t="s">
-        <v>239</v>
+        <v>384</v>
       </c>
       <c r="B95" s="0">
         <v>7.7160493827160446</v>
@@ -1661,7 +2098,7 @@
     </row>
     <row r="96">
       <c r="A96" s="0" t="s">
-        <v>240</v>
+        <v>385</v>
       </c>
       <c r="B96" s="0">
         <v>0.0074480424928103682</v>
@@ -1669,85 +2106,85 @@
     </row>
     <row r="97">
       <c r="A97" s="0" t="s">
-        <v>241</v>
+        <v>386</v>
       </c>
       <c r="B97" s="0">
-        <v>9.7607977524656776e-07</v>
+        <v>9.7607977524390279e-07</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="s">
-        <v>242</v>
+        <v>387</v>
       </c>
       <c r="B98" s="0">
-        <v>0.00024856136270523722</v>
+        <v>0.0002485613627045314</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="s">
-        <v>243</v>
+        <v>388</v>
       </c>
       <c r="B99" s="0">
-        <v>0.078768951651839933</v>
+        <v>0.078768951651781674</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="s">
-        <v>244</v>
+        <v>389</v>
       </c>
       <c r="B100" s="0">
-        <v>0.038269222213323954</v>
+        <v>0.038269222213328603</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="s">
-        <v>245</v>
+        <v>390</v>
       </c>
       <c r="B101" s="0">
-        <v>0.03904170440877501</v>
+        <v>0.039041704408733988</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="s">
-        <v>246</v>
+        <v>391</v>
       </c>
       <c r="B102" s="0">
-        <v>0.068715369703466367</v>
+        <v>0.068715369703414797</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="s">
-        <v>247</v>
+        <v>392</v>
       </c>
       <c r="B103" s="0">
-        <v>0.15316476966791401</v>
+        <v>0.15316476966802273</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="s">
-        <v>248</v>
+        <v>393</v>
       </c>
       <c r="B104" s="0">
-        <v>0.17097285086445771</v>
+        <v>0.1709728508642413</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="s">
-        <v>249</v>
+        <v>394</v>
       </c>
       <c r="B105" s="0">
-        <v>0.23417190063353144</v>
+        <v>0.23417190063359494</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="s">
-        <v>250</v>
+        <v>395</v>
       </c>
       <c r="B106" s="0"/>
     </row>
     <row r="107">
       <c r="A107" s="0" t="s">
-        <v>251</v>
+        <v>396</v>
       </c>
       <c r="B107" s="0">
         <v>1</v>
@@ -1755,7 +2192,7 @@
     </row>
     <row r="108">
       <c r="A108" s="0" t="s">
-        <v>252</v>
+        <v>397</v>
       </c>
       <c r="B108" s="0">
         <v>0.0025000000000000001</v>
@@ -1763,7 +2200,7 @@
     </row>
     <row r="109">
       <c r="A109" s="0" t="s">
-        <v>253</v>
+        <v>398</v>
       </c>
       <c r="B109" s="0">
         <v>0.0070000000000000001</v>
@@ -1771,7 +2208,7 @@
     </row>
     <row r="110">
       <c r="A110" s="0" t="s">
-        <v>254</v>
+        <v>399</v>
       </c>
       <c r="B110" s="0">
         <v>0.0050000000000000001</v>
@@ -1779,7 +2216,7 @@
     </row>
     <row r="111">
       <c r="A111" s="0" t="s">
-        <v>255</v>
+        <v>400</v>
       </c>
       <c r="B111" s="0" t="b">
         <v>0</v>
@@ -1787,7 +2224,7 @@
     </row>
     <row r="112">
       <c r="A112" s="0" t="s">
-        <v>256</v>
+        <v>401</v>
       </c>
       <c r="B112" s="0">
         <v>20</v>
@@ -1795,7 +2232,7 @@
     </row>
     <row r="113">
       <c r="A113" s="0" t="s">
-        <v>257</v>
+        <v>402</v>
       </c>
       <c r="B113" s="0">
         <v>500</v>
@@ -1803,7 +2240,7 @@
     </row>
     <row r="114">
       <c r="A114" s="0" t="s">
-        <v>258</v>
+        <v>403</v>
       </c>
       <c r="B114" s="0">
         <v>0</v>
@@ -1811,7 +2248,7 @@
     </row>
     <row r="115">
       <c r="A115" s="0" t="s">
-        <v>259</v>
+        <v>404</v>
       </c>
       <c r="B115" s="0">
         <v>1</v>
@@ -1819,7 +2256,7 @@
     </row>
     <row r="116">
       <c r="A116" s="0" t="s">
-        <v>260</v>
+        <v>405</v>
       </c>
       <c r="B116" s="0">
         <v>67131.732999999993</v>
@@ -1827,101 +2264,101 @@
     </row>
     <row r="117">
       <c r="A117" s="0" t="s">
-        <v>261</v>
+        <v>406</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>289</v>
+        <v>434</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="s">
-        <v>262</v>
+        <v>407</v>
       </c>
       <c r="B118" s="0"/>
     </row>
     <row r="119">
       <c r="A119" s="0" t="s">
-        <v>263</v>
+        <v>408</v>
       </c>
       <c r="B119" s="0">
-        <v>0.99807122503551482</v>
+        <v>0.9980712250355197</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="s">
-        <v>264</v>
+        <v>409</v>
       </c>
       <c r="B120" s="0">
-        <v>0.99815093150226897</v>
+        <v>0.99815093150227363</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="s">
-        <v>265</v>
+        <v>410</v>
       </c>
       <c r="B121" s="0">
-        <v>0.99823442798099038</v>
+        <v>0.99823442798099482</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="s">
-        <v>266</v>
+        <v>411</v>
       </c>
       <c r="B122" s="0">
-        <v>0.99841045292317909</v>
+        <v>0.99841045292318309</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="s">
-        <v>267</v>
+        <v>412</v>
       </c>
       <c r="B123" s="0">
-        <v>0.99896869870689953</v>
+        <v>0.99896869870690197</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="s">
-        <v>268</v>
+        <v>413</v>
       </c>
       <c r="B124" s="0">
-        <v>0.99971911206486885</v>
+        <v>0.99971911206486919</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="s">
-        <v>269</v>
+        <v>414</v>
       </c>
       <c r="B125" s="0">
-        <v>0.99819137480428144</v>
+        <v>0.99819137480428599</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="s">
-        <v>270</v>
+        <v>415</v>
       </c>
       <c r="B126" s="0">
-        <v>0.99831929933771513</v>
+        <v>0.99831929933771935</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="s">
-        <v>271</v>
+        <v>416</v>
       </c>
       <c r="B127" s="0">
-        <v>0.99859074463950659</v>
+        <v>0.99859074463951003</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="s">
-        <v>272</v>
+        <v>417</v>
       </c>
       <c r="B128" s="0">
-        <v>0.99939074536087336</v>
+        <v>0.99939074536087469</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="s">
-        <v>273</v>
+        <v>418</v>
       </c>
       <c r="B129" s="0">
         <v>0.99986378096829587</v>
@@ -1929,106 +2366,106 @@
     </row>
     <row r="130">
       <c r="A130" s="0" t="s">
-        <v>274</v>
+        <v>419</v>
       </c>
       <c r="B130" s="0">
-        <v>0.057975929798338072</v>
+        <v>0.057975929798377145</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="s">
-        <v>275</v>
+        <v>420</v>
       </c>
       <c r="B131" s="0">
-        <v>0.11079385015254392</v>
+        <v>0.11079385015259076</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="s">
-        <v>276</v>
+        <v>421</v>
       </c>
       <c r="B132" s="0">
-        <v>0.15309827743480539</v>
+        <v>0.15309827743485507</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="s">
-        <v>277</v>
+        <v>422</v>
       </c>
       <c r="B133" s="0">
-        <v>0.20238191941873071</v>
+        <v>0.20238191941876738</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="s">
-        <v>278</v>
+        <v>423</v>
       </c>
       <c r="B134" s="0">
-        <v>0.3141742214749661</v>
+        <v>0.31417422147495727</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="s">
-        <v>279</v>
+        <v>424</v>
       </c>
       <c r="B135" s="0">
-        <v>0.3514654971591018</v>
+        <v>0.35146549715907216</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="s">
-        <v>280</v>
+        <v>425</v>
       </c>
       <c r="B136" s="0">
-        <v>0.13418088908197923</v>
+        <v>0.13418088908202883</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="s">
-        <v>281</v>
+        <v>426</v>
       </c>
       <c r="B137" s="0">
-        <v>0.1779417640403963</v>
+        <v>0.17794176404044004</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="s">
-        <v>282</v>
+        <v>427</v>
       </c>
       <c r="B138" s="0">
-        <v>0.24537555360913288</v>
+        <v>0.24537555360915467</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="s">
-        <v>283</v>
+        <v>428</v>
       </c>
       <c r="B139" s="0">
-        <v>0.35110762370224557</v>
+        <v>0.35110762370221615</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="s">
-        <v>284</v>
+        <v>429</v>
       </c>
       <c r="B140" s="0">
-        <v>0.35152303536270996</v>
+        <v>0.35152303536268009</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="s">
-        <v>285</v>
+        <v>430</v>
       </c>
       <c r="B141" s="0">
-        <v>0.15509140315553227</v>
+        <v>0.15509140315558353</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="s">
-        <v>286</v>
+        <v>431</v>
       </c>
       <c r="B142" s="0">
-        <v>0.097357261221652017</v>
+        <v>0.097357261221693331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
menu cost seems to be working but slow
</commit_message>
<xml_diff>
--- a/output/run3_table.xlsx
+++ b/output/run3_table.xlsx
@@ -13,7 +13,1312 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="870">
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>beta (annualized)</t>
+  </si>
+  <si>
+    <t>____Income Statistics</t>
+  </si>
+  <si>
+    <t>Mean gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log net annual income</t>
+  </si>
+  <si>
+    <t>____Wealth Statistics</t>
+  </si>
+  <si>
+    <t>Mean total wealth</t>
+  </si>
+  <si>
+    <t>Mean liquid wealth</t>
+  </si>
+  <si>
+    <t>w, median</t>
+  </si>
+  <si>
+    <t>b, median</t>
+  </si>
+  <si>
+    <t>s = 0</t>
+  </si>
+  <si>
+    <t>b &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 15% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= $500</t>
+  </si>
+  <si>
+    <t>b &lt;= $1000</t>
+  </si>
+  <si>
+    <t>b &lt;= $2000</t>
+  </si>
+  <si>
+    <t>b &lt;= $5000</t>
+  </si>
+  <si>
+    <t>b &lt;= $10000</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/6</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/12</t>
+  </si>
+  <si>
+    <t>w, Top 10% share</t>
+  </si>
+  <si>
+    <t>w, Top 1% share</t>
+  </si>
+  <si>
+    <t>Gini coefficient, wealth</t>
+  </si>
+  <si>
+    <t>____MPC size effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____MPC sign effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>____MPC for HtM households</t>
+  </si>
+  <si>
+    <t>Quarterly  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>____Wealth percentiles</t>
+  </si>
+  <si>
+    <t>w, 10th pctile</t>
+  </si>
+  <si>
+    <t>w, 25th pctile</t>
+  </si>
+  <si>
+    <t>w, 50th pctile</t>
+  </si>
+  <si>
+    <t>w, 90th pctile</t>
+  </si>
+  <si>
+    <t>w, 95th pctile</t>
+  </si>
+  <si>
+    <t>w, 98th pctile</t>
+  </si>
+  <si>
+    <t>w, 99th pctile</t>
+  </si>
+  <si>
+    <t>w, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Liquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>b, 10th pctile</t>
+  </si>
+  <si>
+    <t>b, 25th pctile</t>
+  </si>
+  <si>
+    <t>b, 50th pctile</t>
+  </si>
+  <si>
+    <t>b, 90th pctile</t>
+  </si>
+  <si>
+    <t>b, 95th pctile</t>
+  </si>
+  <si>
+    <t>b, 98th pctile</t>
+  </si>
+  <si>
+    <t>b, 99th pctile</t>
+  </si>
+  <si>
+    <t>b, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>a, 10th pctile</t>
+  </si>
+  <si>
+    <t>a, 25th pctile</t>
+  </si>
+  <si>
+    <t>a, 50th pctile</t>
+  </si>
+  <si>
+    <t>a, 90th pctile</t>
+  </si>
+  <si>
+    <t>a, 95th pctile</t>
+  </si>
+  <si>
+    <t>a, 98th pctile</t>
+  </si>
+  <si>
+    <t>a, 99th pctile</t>
+  </si>
+  <si>
+    <t>a, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid mpcs</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____Adjustment cost statistics,cost(d,a) =k0 * |d| + k1 * |d| ^ (1 + k2) / (1 + k2)</t>
+  </si>
+  <si>
+    <t>kappa0, adj cost coeff on first (linear) term</t>
+  </si>
+  <si>
+    <t>kappa1, adj cost coeff on second (power) term</t>
+  </si>
+  <si>
+    <t>kappa2, power on second term</t>
+  </si>
+  <si>
+    <t>kappa1 ^(-1/kappa2), low values cause mass at high a</t>
+  </si>
+  <si>
+    <t>a_lb, parameter s.t. max(a, a_lb) used for adj cost</t>
+  </si>
+  <si>
+    <t>Mean adjustment cost, E[chi(d, a)]</t>
+  </si>
+  <si>
+    <t>Mean ratio of deposits to assets, E[|d| / max(a, a_lb)]</t>
+  </si>
+  <si>
+    <t>E[chi(d,a)/abs(d) | d != 0]</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 10th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 25th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 50th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 90th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 95th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 99th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>____Other parameters</t>
+  </si>
+  <si>
+    <t>Experiment group no.</t>
+  </si>
+  <si>
+    <t>Liquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Illiquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Death rate (quarterly)</t>
+  </si>
+  <si>
+    <t>Bequests, on or off</t>
+  </si>
+  <si>
+    <t>Max liquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Max illiquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Borrowing limit</t>
+  </si>
+  <si>
+    <t>CRRA coefficient</t>
+  </si>
+  <si>
+    <t>Value of the numeraire, mean annual earning, in $</t>
+  </si>
+  <si>
+    <t>Income Process</t>
+  </si>
+  <si>
+    <t>____Other statistics</t>
+  </si>
+  <si>
+    <t>a &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= $500</t>
+  </si>
+  <si>
+    <t>a &lt;= $1000</t>
+  </si>
+  <si>
+    <t>a &lt;= $2000</t>
+  </si>
+  <si>
+    <t>a &lt;= $5000</t>
+  </si>
+  <si>
+    <t>a &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= $500</t>
+  </si>
+  <si>
+    <t>w &lt;= $1000</t>
+  </si>
+  <si>
+    <t>w &lt;= $2000</t>
+  </si>
+  <si>
+    <t>w &lt;= $5000</t>
+  </si>
+  <si>
+    <t>w &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>Specification1</t>
+  </si>
+  <si>
+    <t>iy=1, kappa2=0.25</t>
+  </si>
+  <si>
+    <t>cont_a, no meas err</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>beta (annualized)</t>
+  </si>
+  <si>
+    <t>____Income Statistics</t>
+  </si>
+  <si>
+    <t>Mean gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log net annual income</t>
+  </si>
+  <si>
+    <t>____Wealth Statistics</t>
+  </si>
+  <si>
+    <t>Mean total wealth</t>
+  </si>
+  <si>
+    <t>Mean liquid wealth</t>
+  </si>
+  <si>
+    <t>w, median</t>
+  </si>
+  <si>
+    <t>b, median</t>
+  </si>
+  <si>
+    <t>s = 0</t>
+  </si>
+  <si>
+    <t>b &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 15% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= $500</t>
+  </si>
+  <si>
+    <t>b &lt;= $1000</t>
+  </si>
+  <si>
+    <t>b &lt;= $2000</t>
+  </si>
+  <si>
+    <t>b &lt;= $5000</t>
+  </si>
+  <si>
+    <t>b &lt;= $10000</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/6</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/12</t>
+  </si>
+  <si>
+    <t>w, Top 10% share</t>
+  </si>
+  <si>
+    <t>w, Top 1% share</t>
+  </si>
+  <si>
+    <t>Gini coefficient, wealth</t>
+  </si>
+  <si>
+    <t>____MPC size effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____MPC sign effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>____MPC for HtM households</t>
+  </si>
+  <si>
+    <t>Quarterly  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>____Wealth percentiles</t>
+  </si>
+  <si>
+    <t>w, 10th pctile</t>
+  </si>
+  <si>
+    <t>w, 25th pctile</t>
+  </si>
+  <si>
+    <t>w, 50th pctile</t>
+  </si>
+  <si>
+    <t>w, 90th pctile</t>
+  </si>
+  <si>
+    <t>w, 95th pctile</t>
+  </si>
+  <si>
+    <t>w, 98th pctile</t>
+  </si>
+  <si>
+    <t>w, 99th pctile</t>
+  </si>
+  <si>
+    <t>w, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Liquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>b, 10th pctile</t>
+  </si>
+  <si>
+    <t>b, 25th pctile</t>
+  </si>
+  <si>
+    <t>b, 50th pctile</t>
+  </si>
+  <si>
+    <t>b, 90th pctile</t>
+  </si>
+  <si>
+    <t>b, 95th pctile</t>
+  </si>
+  <si>
+    <t>b, 98th pctile</t>
+  </si>
+  <si>
+    <t>b, 99th pctile</t>
+  </si>
+  <si>
+    <t>b, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>a, 10th pctile</t>
+  </si>
+  <si>
+    <t>a, 25th pctile</t>
+  </si>
+  <si>
+    <t>a, 50th pctile</t>
+  </si>
+  <si>
+    <t>a, 90th pctile</t>
+  </si>
+  <si>
+    <t>a, 95th pctile</t>
+  </si>
+  <si>
+    <t>a, 98th pctile</t>
+  </si>
+  <si>
+    <t>a, 99th pctile</t>
+  </si>
+  <si>
+    <t>a, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid mpcs</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____Adjustment cost statistics,cost(d,a) =k0 * |d| + k1 * |d| ^ (1 + k2) / (1 + k2)</t>
+  </si>
+  <si>
+    <t>kappa0, adj cost coeff on first (linear) term</t>
+  </si>
+  <si>
+    <t>kappa1, adj cost coeff on second (power) term</t>
+  </si>
+  <si>
+    <t>kappa2, power on second term</t>
+  </si>
+  <si>
+    <t>kappa1 ^(-1/kappa2), low values cause mass at high a</t>
+  </si>
+  <si>
+    <t>a_lb, parameter s.t. max(a, a_lb) used for adj cost</t>
+  </si>
+  <si>
+    <t>Mean adjustment cost, E[chi(d, a)]</t>
+  </si>
+  <si>
+    <t>Mean ratio of deposits to assets, E[|d| / max(a, a_lb)]</t>
+  </si>
+  <si>
+    <t>E[chi(d,a)/abs(d) | d != 0]</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 10th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 25th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 50th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 90th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 95th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 99th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>____Other parameters</t>
+  </si>
+  <si>
+    <t>Experiment group no.</t>
+  </si>
+  <si>
+    <t>Liquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Illiquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Death rate (quarterly)</t>
+  </si>
+  <si>
+    <t>Bequests, on or off</t>
+  </si>
+  <si>
+    <t>Max liquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Max illiquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Borrowing limit</t>
+  </si>
+  <si>
+    <t>CRRA coefficient</t>
+  </si>
+  <si>
+    <t>Value of the numeraire, mean annual earning, in $</t>
+  </si>
+  <si>
+    <t>Income Process</t>
+  </si>
+  <si>
+    <t>____Other statistics</t>
+  </si>
+  <si>
+    <t>a &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= $500</t>
+  </si>
+  <si>
+    <t>a &lt;= $1000</t>
+  </si>
+  <si>
+    <t>a &lt;= $2000</t>
+  </si>
+  <si>
+    <t>a &lt;= $5000</t>
+  </si>
+  <si>
+    <t>a &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= $500</t>
+  </si>
+  <si>
+    <t>w &lt;= $1000</t>
+  </si>
+  <si>
+    <t>w &lt;= $2000</t>
+  </si>
+  <si>
+    <t>w &lt;= $5000</t>
+  </si>
+  <si>
+    <t>w &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>Specification1</t>
+  </si>
+  <si>
+    <t>iy=1, kappa2=0.25</t>
+  </si>
+  <si>
+    <t>cont_a, no meas err</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>beta (annualized)</t>
+  </si>
+  <si>
+    <t>____Income Statistics</t>
+  </si>
+  <si>
+    <t>Mean gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log net annual income</t>
+  </si>
+  <si>
+    <t>____Wealth Statistics</t>
+  </si>
+  <si>
+    <t>Mean total wealth</t>
+  </si>
+  <si>
+    <t>Mean liquid wealth</t>
+  </si>
+  <si>
+    <t>w, median</t>
+  </si>
+  <si>
+    <t>b, median</t>
+  </si>
+  <si>
+    <t>s = 0</t>
+  </si>
+  <si>
+    <t>b &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 15% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= $500</t>
+  </si>
+  <si>
+    <t>b &lt;= $1000</t>
+  </si>
+  <si>
+    <t>b &lt;= $2000</t>
+  </si>
+  <si>
+    <t>b &lt;= $5000</t>
+  </si>
+  <si>
+    <t>b &lt;= $10000</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/6</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/12</t>
+  </si>
+  <si>
+    <t>w, Top 10% share</t>
+  </si>
+  <si>
+    <t>w, Top 1% share</t>
+  </si>
+  <si>
+    <t>Gini coefficient, wealth</t>
+  </si>
+  <si>
+    <t>____MPC size effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____MPC sign effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>____MPC for HtM households</t>
+  </si>
+  <si>
+    <t>Quarterly  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>____Wealth percentiles</t>
+  </si>
+  <si>
+    <t>w, 10th pctile</t>
+  </si>
+  <si>
+    <t>w, 25th pctile</t>
+  </si>
+  <si>
+    <t>w, 50th pctile</t>
+  </si>
+  <si>
+    <t>w, 90th pctile</t>
+  </si>
+  <si>
+    <t>w, 95th pctile</t>
+  </si>
+  <si>
+    <t>w, 98th pctile</t>
+  </si>
+  <si>
+    <t>w, 99th pctile</t>
+  </si>
+  <si>
+    <t>w, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Liquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>b, 10th pctile</t>
+  </si>
+  <si>
+    <t>b, 25th pctile</t>
+  </si>
+  <si>
+    <t>b, 50th pctile</t>
+  </si>
+  <si>
+    <t>b, 90th pctile</t>
+  </si>
+  <si>
+    <t>b, 95th pctile</t>
+  </si>
+  <si>
+    <t>b, 98th pctile</t>
+  </si>
+  <si>
+    <t>b, 99th pctile</t>
+  </si>
+  <si>
+    <t>b, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>a, 10th pctile</t>
+  </si>
+  <si>
+    <t>a, 25th pctile</t>
+  </si>
+  <si>
+    <t>a, 50th pctile</t>
+  </si>
+  <si>
+    <t>a, 90th pctile</t>
+  </si>
+  <si>
+    <t>a, 95th pctile</t>
+  </si>
+  <si>
+    <t>a, 98th pctile</t>
+  </si>
+  <si>
+    <t>a, 99th pctile</t>
+  </si>
+  <si>
+    <t>a, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid mpcs</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____Adjustment cost statistics,cost(d,a) =k0 * |d| + k1 * |d| ^ (1 + k2) / (1 + k2)</t>
+  </si>
+  <si>
+    <t>kappa0, adj cost coeff on first (linear) term</t>
+  </si>
+  <si>
+    <t>kappa1, adj cost coeff on second (power) term</t>
+  </si>
+  <si>
+    <t>kappa2, power on second term</t>
+  </si>
+  <si>
+    <t>kappa1 ^(-1/kappa2), low values cause mass at high a</t>
+  </si>
+  <si>
+    <t>a_lb, parameter s.t. max(a, a_lb) used for adj cost</t>
+  </si>
+  <si>
+    <t>Mean adjustment cost, E[chi(d, a)]</t>
+  </si>
+  <si>
+    <t>Mean ratio of deposits to assets, E[|d| / max(a, a_lb)]</t>
+  </si>
+  <si>
+    <t>E[chi(d,a)/abs(d) | d != 0]</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 10th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 25th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 50th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 90th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 95th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 99th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>____Other parameters</t>
+  </si>
+  <si>
+    <t>Experiment group no.</t>
+  </si>
+  <si>
+    <t>Liquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Illiquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Death rate (quarterly)</t>
+  </si>
+  <si>
+    <t>Bequests, on or off</t>
+  </si>
+  <si>
+    <t>Max liquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Max illiquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Borrowing limit</t>
+  </si>
+  <si>
+    <t>CRRA coefficient</t>
+  </si>
+  <si>
+    <t>Value of the numeraire, mean annual earning, in $</t>
+  </si>
+  <si>
+    <t>Income Process</t>
+  </si>
+  <si>
+    <t>____Other statistics</t>
+  </si>
+  <si>
+    <t>a &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= $500</t>
+  </si>
+  <si>
+    <t>a &lt;= $1000</t>
+  </si>
+  <si>
+    <t>a &lt;= $2000</t>
+  </si>
+  <si>
+    <t>a &lt;= $5000</t>
+  </si>
+  <si>
+    <t>a &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= $500</t>
+  </si>
+  <si>
+    <t>w &lt;= $1000</t>
+  </si>
+  <si>
+    <t>w &lt;= $2000</t>
+  </si>
+  <si>
+    <t>w &lt;= $5000</t>
+  </si>
+  <si>
+    <t>w &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>Specification1</t>
+  </si>
+  <si>
+    <t>iy=1, kappa2=0.25</t>
+  </si>
+  <si>
+    <t>cont_a, no meas err</t>
+  </si>
   <si>
     <t>Row</t>
   </si>
@@ -1338,7 +2643,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1349,15 +2654,21 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1376,39 +2687,39 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>290</v>
+        <v>725</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>432</v>
+        <v>867</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>291</v>
+        <v>726</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>433</v>
+        <v>868</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>292</v>
+        <v>727</v>
       </c>
       <c r="B3" s="0">
-        <v>8.7285132994264512</v>
+        <v>9.116719384541657</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>293</v>
+        <v>728</v>
       </c>
       <c r="B4" s="0">
-        <v>23.920912670566707</v>
+        <v>24.99010225758682</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>294</v>
+        <v>729</v>
       </c>
       <c r="B5" s="0">
         <v>0.98019867330675525</v>
@@ -1416,13 +2727,13 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>295</v>
+        <v>730</v>
       </c>
       <c r="B6" s="0"/>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>296</v>
+        <v>731</v>
       </c>
       <c r="B7" s="0">
         <v>1.0691087245941162</v>
@@ -1430,7 +2741,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>297</v>
+        <v>732</v>
       </c>
       <c r="B8" s="0">
         <v>0.77865374088287354</v>
@@ -1438,7 +2749,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>298</v>
+        <v>733</v>
       </c>
       <c r="B9" s="0">
         <v>0.77865374088287354</v>
@@ -1446,497 +2757,497 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>299</v>
+        <v>734</v>
       </c>
       <c r="B10" s="0"/>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>300</v>
+        <v>735</v>
       </c>
       <c r="B11" s="0">
-        <v>0.81138036092356036</v>
+        <v>1.3015100465134124</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>301</v>
+        <v>736</v>
       </c>
       <c r="B12" s="0">
-        <v>0.81088099507740774</v>
+        <v>0.45163136922346869</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>302</v>
+        <v>737</v>
       </c>
       <c r="B13" s="0">
-        <v>0.22694281077739129</v>
+        <v>0.5675184511539596</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>303</v>
+        <v>738</v>
       </c>
       <c r="B14" s="0">
-        <v>0.18989735697904642</v>
+        <v>0.24980322077849007</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>304</v>
+        <v>739</v>
       </c>
       <c r="B15" s="0">
-        <v>0.23749110138386587</v>
+        <v>0.079094685911616447</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>305</v>
+        <v>740</v>
       </c>
       <c r="B16" s="0">
-        <v>0.057989368858519096</v>
+        <v>0.022211829135925738</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>306</v>
+        <v>741</v>
       </c>
       <c r="B17" s="0">
-        <v>0.11082803850547124</v>
+        <v>0.057183761737173454</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>307</v>
+        <v>742</v>
       </c>
       <c r="B18" s="0">
-        <v>0.15314978285992428</v>
+        <v>0.071426442695460585</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>308</v>
+        <v>743</v>
       </c>
       <c r="B19" s="0">
-        <v>0.20042031734194862</v>
+        <v>0.097309553577737323</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>309</v>
+        <v>744</v>
       </c>
       <c r="B20" s="0">
-        <v>0.29728632729763427</v>
+        <v>0.1737315807428475</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>310</v>
+        <v>745</v>
       </c>
       <c r="B21" s="0">
-        <v>0.39040564336825689</v>
+        <v>0.27466990196666585</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>311</v>
+        <v>746</v>
       </c>
       <c r="B22" s="0">
-        <v>0.45969393975673728</v>
+        <v>0.36041667475797562</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>312</v>
+        <v>747</v>
       </c>
       <c r="B23" s="0">
-        <v>0.1342244050893541</v>
+        <v>0.064326298766569062</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>313</v>
+        <v>748</v>
       </c>
       <c r="B24" s="0">
-        <v>0.17754458123368744</v>
+        <v>0.08440079858825654</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>314</v>
+        <v>749</v>
       </c>
       <c r="B25" s="0">
-        <v>0.23842040534140532</v>
+        <v>0.12371663375213646</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>315</v>
+        <v>750</v>
       </c>
       <c r="B26" s="0">
-        <v>0.34708921160906692</v>
+        <v>0.22541030383281818</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>316</v>
+        <v>751</v>
       </c>
       <c r="B27" s="0">
-        <v>0.45843989528414586</v>
+        <v>0.35876170596305312</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>317</v>
+        <v>752</v>
       </c>
       <c r="B28" s="0">
-        <v>0.1561082630159637</v>
+        <v>0.086056841611374099</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>318</v>
+        <v>753</v>
       </c>
       <c r="B29" s="0">
-        <v>0.098206497818401323</v>
+        <v>0.061475902060985015</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>319</v>
+        <v>754</v>
       </c>
       <c r="B30" s="0">
-        <v>0.0065138118939686018</v>
+        <v>0.36295204655549029</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>320</v>
+        <v>755</v>
       </c>
       <c r="B31" s="0">
-        <v>0.0086474583207147848</v>
+        <v>0.39922846162625314</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>321</v>
+        <v>756</v>
       </c>
       <c r="B32" s="0">
-        <v>0.49770029962151197</v>
+        <v>0.45878030033091588</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>322</v>
+        <v>757</v>
       </c>
       <c r="B33" s="0">
-        <v>0.10903998460942077</v>
+        <v>0.094571343301446231</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>323</v>
+        <v>758</v>
       </c>
       <c r="B34" s="0">
-        <v>0.67019544887908689</v>
+        <v>0.63797903578719728</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>324</v>
+        <v>759</v>
       </c>
       <c r="B35" s="0"/>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>325</v>
+        <v>760</v>
       </c>
       <c r="B36" s="0">
-        <v>8.7285132994463588</v>
+        <v>9.640499803104051</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>326</v>
+        <v>761</v>
       </c>
       <c r="B37" s="0">
-        <v>7.0820274460317743</v>
+        <v>7.5068121152362943</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>327</v>
+        <v>762</v>
       </c>
       <c r="B38" s="0">
-        <v>23.920912670588404</v>
+        <v>25.187338263721852</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>328</v>
+        <v>763</v>
       </c>
       <c r="B39" s="0">
-        <v>22.524652684370228</v>
+        <v>23.52529456422824</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>329</v>
+        <v>764</v>
       </c>
       <c r="B40" s="0"/>
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>330</v>
+        <v>765</v>
       </c>
       <c r="B41" s="0">
-        <v>15.622825160200909</v>
+        <v>11.419268244456651</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>331</v>
+        <v>766</v>
       </c>
       <c r="B42" s="0">
-        <v>15.622825160195298</v>
+        <v>12.410737817076134</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>332</v>
+        <v>767</v>
       </c>
       <c r="B43" s="0">
-        <v>21.500324605083986</v>
+        <v>18.645395983645702</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>333</v>
+        <v>768</v>
       </c>
       <c r="B44" s="0">
-        <v>33.741782519713013</v>
+        <v>28.295106983530395</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>334</v>
+        <v>769</v>
       </c>
       <c r="B45" s="0">
-        <v>33.741782519700969</v>
+        <v>28.992480113686568</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>335</v>
+        <v>770</v>
       </c>
       <c r="B46" s="0">
-        <v>36.88196131884856</v>
+        <v>33.419330541784014</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>336</v>
+        <v>771</v>
       </c>
       <c r="B47" s="0"/>
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>337</v>
+        <v>772</v>
       </c>
       <c r="B48" s="0">
-        <v>28.679518103847833</v>
+        <v>39.079543442838016</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>338</v>
+        <v>773</v>
       </c>
       <c r="B49" s="0">
-        <v>28.287209478128812</v>
+        <v>33.015552175839346</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>339</v>
+        <v>774</v>
       </c>
       <c r="B50" s="0">
-        <v>28.679690573816398</v>
+        <v>42.565807672304651</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>340</v>
+        <v>775</v>
       </c>
       <c r="B51" s="0">
-        <v>53.296321179570924</v>
+        <v>60.619883724315692</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>341</v>
+        <v>776</v>
       </c>
       <c r="B52" s="0">
-        <v>51.898352806477966</v>
+        <v>48.691057560820788</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>342</v>
+        <v>777</v>
       </c>
       <c r="B53" s="0">
-        <v>53.296935766010137</v>
+        <v>67.477914701313054</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>343</v>
+        <v>778</v>
       </c>
       <c r="B54" s="0"/>
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>344</v>
+        <v>779</v>
       </c>
       <c r="B55" s="0">
-        <v>0.0029635246545148494</v>
+        <v>0.039107399303962974</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>345</v>
+        <v>780</v>
       </c>
       <c r="B56" s="0">
-        <v>0.021869294845328346</v>
+        <v>0.14413513933202654</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>346</v>
+        <v>781</v>
       </c>
       <c r="B57" s="0">
-        <v>0.22694281077739129</v>
+        <v>0.5675184511539596</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>347</v>
+        <v>782</v>
       </c>
       <c r="B58" s="0">
-        <v>1.743083423750011</v>
+        <v>3.4309604039847126</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>348</v>
+        <v>783</v>
       </c>
       <c r="B59" s="0">
-        <v>2.7389698883246605</v>
+        <v>5.1365321085388755</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>349</v>
+        <v>784</v>
       </c>
       <c r="B60" s="0">
-        <v>5.5530515937904967</v>
+        <v>7.4852298291134511</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>350</v>
+        <v>785</v>
       </c>
       <c r="B61" s="0">
-        <v>5.6482333471432691</v>
+        <v>9.3362364059277141</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>351</v>
+        <v>786</v>
       </c>
       <c r="B62" s="0">
-        <v>12.859337972504475</v>
+        <v>16.221704138949644</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
-        <v>352</v>
+        <v>787</v>
       </c>
       <c r="B63" s="0"/>
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
-        <v>353</v>
+        <v>788</v>
       </c>
       <c r="B64" s="0">
-        <v>0.0029606024109443954</v>
+        <v>0.021035551995870705</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
-        <v>354</v>
+        <v>789</v>
       </c>
       <c r="B65" s="0">
-        <v>0.034326090628109804</v>
+        <v>0.086934706747243018</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">
-        <v>355</v>
+        <v>790</v>
       </c>
       <c r="B66" s="0">
-        <v>0.18989735697904642</v>
+        <v>0.24980322077849007</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="s">
-        <v>356</v>
+        <v>791</v>
       </c>
       <c r="B67" s="0">
-        <v>1.7247213493765416</v>
+        <v>0.95293865112936205</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
-        <v>357</v>
+        <v>792</v>
       </c>
       <c r="B68" s="0">
-        <v>2.7281765775996458</v>
+        <v>1.3295879202395846</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="s">
-        <v>358</v>
+        <v>793</v>
       </c>
       <c r="B69" s="0">
-        <v>4.2636404013217497</v>
+        <v>1.903979927044207</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="s">
-        <v>359</v>
+        <v>794</v>
       </c>
       <c r="B70" s="0">
-        <v>5.5685675406640334</v>
+        <v>2.4101473909231936</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="s">
-        <v>360</v>
+        <v>795</v>
       </c>
       <c r="B71" s="0">
-        <v>10.269739239515749</v>
+        <v>4.6016565934170544</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
-        <v>361</v>
+        <v>796</v>
       </c>
       <c r="B72" s="0"/>
     </row>
     <row r="73">
       <c r="A73" s="0" t="s">
-        <v>362</v>
+        <v>797</v>
       </c>
       <c r="B73" s="0">
         <v>0</v>
@@ -1944,7 +3255,7 @@
     </row>
     <row r="74">
       <c r="A74" s="0" t="s">
-        <v>363</v>
+        <v>798</v>
       </c>
       <c r="B74" s="0">
         <v>0</v>
@@ -1952,121 +3263,121 @@
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
-        <v>364</v>
+        <v>799</v>
       </c>
       <c r="B75" s="0">
-        <v>0</v>
+        <v>0.13212404702681962</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
-        <v>365</v>
+        <v>800</v>
       </c>
       <c r="B76" s="0">
-        <v>0</v>
+        <v>2.0650637357756376</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
-        <v>366</v>
+        <v>801</v>
       </c>
       <c r="B77" s="0">
-        <v>0</v>
+        <v>3.3199481980525083</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
-        <v>367</v>
+        <v>802</v>
       </c>
       <c r="B78" s="0">
-        <v>0</v>
+        <v>5.1924200068271134</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="s">
-        <v>368</v>
+        <v>803</v>
       </c>
       <c r="B79" s="0">
-        <v>0</v>
+        <v>6.7299363807188293</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="s">
-        <v>369</v>
+        <v>804</v>
       </c>
       <c r="B80" s="0">
-        <v>0.021412439236011851</v>
+        <v>12.507471497288467</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="s">
-        <v>370</v>
+        <v>805</v>
       </c>
       <c r="B81" s="0"/>
     </row>
     <row r="82">
       <c r="A82" s="0" t="s">
-        <v>371</v>
+        <v>806</v>
       </c>
       <c r="B82" s="0"/>
     </row>
     <row r="83">
       <c r="A83" s="0" t="s">
-        <v>372</v>
+        <v>807</v>
       </c>
       <c r="B83" s="0"/>
     </row>
     <row r="84">
       <c r="A84" s="0" t="s">
-        <v>373</v>
+        <v>808</v>
       </c>
       <c r="B84" s="0"/>
     </row>
     <row r="85">
       <c r="A85" s="0" t="s">
-        <v>374</v>
+        <v>809</v>
       </c>
       <c r="B85" s="0"/>
     </row>
     <row r="86">
       <c r="A86" s="0" t="s">
-        <v>375</v>
+        <v>810</v>
       </c>
       <c r="B86" s="0"/>
     </row>
     <row r="87">
       <c r="A87" s="0" t="s">
-        <v>376</v>
+        <v>811</v>
       </c>
       <c r="B87" s="0"/>
     </row>
     <row r="88">
       <c r="A88" s="0" t="s">
-        <v>377</v>
+        <v>812</v>
       </c>
       <c r="B88" s="0"/>
     </row>
     <row r="89">
       <c r="A89" s="0" t="s">
-        <v>378</v>
+        <v>813</v>
       </c>
       <c r="B89" s="0"/>
     </row>
     <row r="90">
       <c r="A90" s="0" t="s">
-        <v>379</v>
+        <v>814</v>
       </c>
       <c r="B90" s="0"/>
     </row>
     <row r="91">
       <c r="A91" s="0" t="s">
-        <v>380</v>
+        <v>815</v>
       </c>
       <c r="B91" s="0"/>
     </row>
     <row r="92">
       <c r="A92" s="0" t="s">
-        <v>381</v>
+        <v>816</v>
       </c>
       <c r="B92" s="0">
         <v>0</v>
@@ -2074,7 +3385,7 @@
     </row>
     <row r="93">
       <c r="A93" s="0" t="s">
-        <v>382</v>
+        <v>817</v>
       </c>
       <c r="B93" s="0">
         <v>0.60000000000000009</v>
@@ -2082,7 +3393,7 @@
     </row>
     <row r="94">
       <c r="A94" s="0" t="s">
-        <v>383</v>
+        <v>818</v>
       </c>
       <c r="B94" s="0">
         <v>0.25</v>
@@ -2090,7 +3401,7 @@
     </row>
     <row r="95">
       <c r="A95" s="0" t="s">
-        <v>384</v>
+        <v>819</v>
       </c>
       <c r="B95" s="0">
         <v>7.7160493827160446</v>
@@ -2098,7 +3409,7 @@
     </row>
     <row r="96">
       <c r="A96" s="0" t="s">
-        <v>385</v>
+        <v>820</v>
       </c>
       <c r="B96" s="0">
         <v>0.0074480424928103682</v>
@@ -2106,85 +3417,85 @@
     </row>
     <row r="97">
       <c r="A97" s="0" t="s">
-        <v>386</v>
+        <v>821</v>
       </c>
       <c r="B97" s="0">
-        <v>9.7607977524390279e-07</v>
+        <v>0.00021438359318827539</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="s">
-        <v>387</v>
+        <v>822</v>
       </c>
       <c r="B98" s="0">
-        <v>0.0002485613627045314</v>
+        <v>0.00089886556379539708</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="s">
-        <v>388</v>
+        <v>823</v>
       </c>
       <c r="B99" s="0">
-        <v>0.078768951651781674</v>
+        <v>0.066778044672193976</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="s">
-        <v>389</v>
+        <v>824</v>
       </c>
       <c r="B100" s="0">
-        <v>0.038269222213328603</v>
+        <v>0.012350027966423356</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="s">
-        <v>390</v>
+        <v>825</v>
       </c>
       <c r="B101" s="0">
-        <v>0.039041704408733988</v>
+        <v>0.018693177156555472</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="s">
-        <v>391</v>
+        <v>826</v>
       </c>
       <c r="B102" s="0">
-        <v>0.068715369703414797</v>
+        <v>0.034932534215827024</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="s">
-        <v>392</v>
+        <v>827</v>
       </c>
       <c r="B103" s="0">
-        <v>0.15316476966802273</v>
+        <v>0.18007141403348462</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="s">
-        <v>393</v>
+        <v>828</v>
       </c>
       <c r="B104" s="0">
-        <v>0.1709728508642413</v>
+        <v>0.23556645926903735</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="s">
-        <v>394</v>
+        <v>829</v>
       </c>
       <c r="B105" s="0">
-        <v>0.23417190063359494</v>
+        <v>0.28367135610621719</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="s">
-        <v>395</v>
+        <v>830</v>
       </c>
       <c r="B106" s="0"/>
     </row>
     <row r="107">
       <c r="A107" s="0" t="s">
-        <v>396</v>
+        <v>831</v>
       </c>
       <c r="B107" s="0">
         <v>1</v>
@@ -2192,7 +3503,7 @@
     </row>
     <row r="108">
       <c r="A108" s="0" t="s">
-        <v>397</v>
+        <v>832</v>
       </c>
       <c r="B108" s="0">
         <v>0.0025000000000000001</v>
@@ -2200,7 +3511,7 @@
     </row>
     <row r="109">
       <c r="A109" s="0" t="s">
-        <v>398</v>
+        <v>833</v>
       </c>
       <c r="B109" s="0">
         <v>0.0070000000000000001</v>
@@ -2208,7 +3519,7 @@
     </row>
     <row r="110">
       <c r="A110" s="0" t="s">
-        <v>399</v>
+        <v>834</v>
       </c>
       <c r="B110" s="0">
         <v>0.0050000000000000001</v>
@@ -2216,7 +3527,7 @@
     </row>
     <row r="111">
       <c r="A111" s="0" t="s">
-        <v>400</v>
+        <v>835</v>
       </c>
       <c r="B111" s="0" t="b">
         <v>0</v>
@@ -2224,7 +3535,7 @@
     </row>
     <row r="112">
       <c r="A112" s="0" t="s">
-        <v>401</v>
+        <v>836</v>
       </c>
       <c r="B112" s="0">
         <v>20</v>
@@ -2232,7 +3543,7 @@
     </row>
     <row r="113">
       <c r="A113" s="0" t="s">
-        <v>402</v>
+        <v>837</v>
       </c>
       <c r="B113" s="0">
         <v>500</v>
@@ -2240,7 +3551,7 @@
     </row>
     <row r="114">
       <c r="A114" s="0" t="s">
-        <v>403</v>
+        <v>838</v>
       </c>
       <c r="B114" s="0">
         <v>0</v>
@@ -2248,7 +3559,7 @@
     </row>
     <row r="115">
       <c r="A115" s="0" t="s">
-        <v>404</v>
+        <v>839</v>
       </c>
       <c r="B115" s="0">
         <v>1</v>
@@ -2256,7 +3567,7 @@
     </row>
     <row r="116">
       <c r="A116" s="0" t="s">
-        <v>405</v>
+        <v>840</v>
       </c>
       <c r="B116" s="0">
         <v>67131.732999999993</v>
@@ -2264,208 +3575,208 @@
     </row>
     <row r="117">
       <c r="A117" s="0" t="s">
-        <v>406</v>
+        <v>841</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>434</v>
+        <v>869</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="s">
-        <v>407</v>
+        <v>842</v>
       </c>
       <c r="B118" s="0"/>
     </row>
     <row r="119">
       <c r="A119" s="0" t="s">
-        <v>408</v>
+        <v>843</v>
       </c>
       <c r="B119" s="0">
-        <v>0.9980712250355197</v>
+        <v>0.44468084681745401</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="s">
-        <v>409</v>
+        <v>844</v>
       </c>
       <c r="B120" s="0">
-        <v>0.99815093150227363</v>
+        <v>0.44580014684530594</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="s">
-        <v>410</v>
+        <v>845</v>
       </c>
       <c r="B121" s="0">
-        <v>0.99823442798099482</v>
+        <v>0.44618576252432707</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="s">
-        <v>411</v>
+        <v>846</v>
       </c>
       <c r="B122" s="0">
-        <v>0.99841045292318309</v>
+        <v>0.44732290390495255</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="s">
-        <v>412</v>
+        <v>847</v>
       </c>
       <c r="B123" s="0">
-        <v>0.99896869870690197</v>
+        <v>0.45842082614099749</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="s">
-        <v>413</v>
+        <v>848</v>
       </c>
       <c r="B124" s="0">
-        <v>0.99971911206486919</v>
+        <v>0.48246202513170738</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="s">
-        <v>414</v>
+        <v>849</v>
       </c>
       <c r="B125" s="0">
-        <v>0.99819137480428599</v>
+        <v>0.44601672694032263</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="s">
-        <v>415</v>
+        <v>850</v>
       </c>
       <c r="B126" s="0">
-        <v>0.99831929933771935</v>
+        <v>0.44655502712315909</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="s">
-        <v>416</v>
+        <v>851</v>
       </c>
       <c r="B127" s="0">
-        <v>0.99859074463951003</v>
+        <v>0.44995866167191068</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="s">
-        <v>417</v>
+        <v>852</v>
       </c>
       <c r="B128" s="0">
-        <v>0.99939074536087469</v>
+        <v>0.46965851691327809</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="s">
-        <v>418</v>
+        <v>853</v>
       </c>
       <c r="B129" s="0">
-        <v>0.99986378096829587</v>
+        <v>0.50962703071267001</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="s">
-        <v>419</v>
+        <v>854</v>
       </c>
       <c r="B130" s="0">
-        <v>0.057975929798377145</v>
+        <v>0.01965419043014115</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="s">
-        <v>420</v>
+        <v>855</v>
       </c>
       <c r="B131" s="0">
-        <v>0.11079385015259076</v>
+        <v>0.030264481788025169</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="s">
-        <v>421</v>
+        <v>856</v>
       </c>
       <c r="B132" s="0">
-        <v>0.15309827743485507</v>
+        <v>0.044335176411717157</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="s">
-        <v>422</v>
+        <v>857</v>
       </c>
       <c r="B133" s="0">
-        <v>0.20238191941876738</v>
+        <v>0.047488791595911767</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="s">
-        <v>423</v>
+        <v>858</v>
       </c>
       <c r="B134" s="0">
-        <v>0.31417422147495727</v>
+        <v>0.11074973781087466</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="s">
-        <v>424</v>
+        <v>859</v>
       </c>
       <c r="B135" s="0">
-        <v>0.35146549715907216</v>
+        <v>0.18556133864327162</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="s">
-        <v>425</v>
+        <v>860</v>
       </c>
       <c r="B136" s="0">
-        <v>0.13418088908202883</v>
+        <v>0.03938861705534933</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="s">
-        <v>426</v>
+        <v>861</v>
       </c>
       <c r="B137" s="0">
-        <v>0.17794176404044004</v>
+        <v>0.044377231993790567</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="s">
-        <v>427</v>
+        <v>862</v>
       </c>
       <c r="B138" s="0">
-        <v>0.24537555360915467</v>
+        <v>0.069440413690089381</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="s">
-        <v>428</v>
+        <v>863</v>
       </c>
       <c r="B139" s="0">
-        <v>0.35110762370221615</v>
+        <v>0.15767197136195391</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="s">
-        <v>429</v>
+        <v>864</v>
       </c>
       <c r="B140" s="0">
-        <v>0.35152303536268009</v>
+        <v>0.25668497432890575</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="s">
-        <v>430</v>
+        <v>865</v>
       </c>
       <c r="B141" s="0">
-        <v>0.15509140315558353</v>
+        <v>0.054822334828424191</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="s">
-        <v>431</v>
+        <v>866</v>
       </c>
       <c r="B142" s="0">
-        <v>0.097357261221693331</v>
+        <v>0.036932972254091763</v>
       </c>
     </row>
   </sheetData>

</xml_diff>